<commit_message>
Excel table Marc Galvez
</commit_message>
<xml_diff>
--- a/P1/AndroDunos_TimeTable.xlsx
+++ b/P1/AndroDunos_TimeTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Christian\proyectosVisual\MyAwesomeGame2\Andro-Dunos-main\P1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UNI\Proyecto 1\Github\Andro-Dunos-main\P1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1703A37-2E37-428D-80E0-EEBB61F1FA2C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D3602896-76EA-4366-AE28-6EEC6E5CA2DD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="14130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -105,9 +105,6 @@
     <t>Fix Player 1 Animation</t>
   </si>
   <si>
-    <t>Stage Clear Score</t>
-  </si>
-  <si>
     <t>Player 2 Module</t>
   </si>
   <si>
@@ -223,6 +220,9 @@
   </si>
   <si>
     <t>Power up bonus</t>
+  </si>
+  <si>
+    <t>Stage Clear Bonus</t>
   </si>
 </sst>
 </file>
@@ -233,7 +233,7 @@
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="165" formatCode="[h]:mm:ss;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,30 +250,18 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -459,109 +447,101 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="46" fontId="1" fillId="4" borderId="4" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="21" fontId="1" fillId="4" borderId="11" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="46" fontId="1" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="1" fillId="3" borderId="11" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="2" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="7" borderId="4" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="6" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="7" borderId="0" xfId="6" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="7" borderId="0" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="6" borderId="4" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="5" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="0" xfId="5" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="0" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="4" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="4" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="8">
-    <cellStyle name="40% - Énfasis1" xfId="3" builtinId="31"/>
-    <cellStyle name="40% - Énfasis2" xfId="6" builtinId="35"/>
-    <cellStyle name="60% - Énfasis1" xfId="4" builtinId="32"/>
-    <cellStyle name="60% - Énfasis2" xfId="7" builtinId="36"/>
-    <cellStyle name="Énfasis1" xfId="2" builtinId="29"/>
-    <cellStyle name="Énfasis2" xfId="5" builtinId="33"/>
-    <cellStyle name="Incorrecto" xfId="1" builtinId="27"/>
+  <cellStyles count="7">
+    <cellStyle name="40% - Énfasis1" xfId="2" builtinId="31"/>
+    <cellStyle name="40% - Énfasis2" xfId="5" builtinId="35"/>
+    <cellStyle name="60% - Énfasis1" xfId="3" builtinId="32"/>
+    <cellStyle name="60% - Énfasis2" xfId="6" builtinId="36"/>
+    <cellStyle name="Énfasis1" xfId="1" builtinId="29"/>
+    <cellStyle name="Énfasis2" xfId="4" builtinId="33"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -843,10 +823,10 @@
   <dimension ref="B1:K56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E62" sqref="E62"/>
+      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,10 +851,10 @@
         <v>5</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>1</v>
@@ -936,7 +916,7 @@
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>13</v>
@@ -1031,13 +1011,17 @@
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="16" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
+      <c r="D10" s="22">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E10" s="22">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="F10" s="19">
         <v>43206</v>
       </c>
@@ -1078,15 +1062,15 @@
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="21">
+      <c r="D13" s="23">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E13" s="21">
+      <c r="E13" s="23">
         <v>3.125E-2</v>
       </c>
       <c r="F13" s="19">
@@ -1117,10 +1101,10 @@
       <c r="C15" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="26">
+      <c r="D15" s="22">
         <v>6.25E-2</v>
       </c>
-      <c r="E15" s="26">
+      <c r="E15" s="22">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F15" s="19">
@@ -1134,10 +1118,10 @@
       <c r="C16" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="22">
+      <c r="D16" s="21">
         <v>0.16666666666666666</v>
       </c>
-      <c r="E16" s="23">
+      <c r="E16" s="22">
         <v>0.20833333333333334</v>
       </c>
       <c r="F16" s="19">
@@ -1151,8 +1135,12 @@
       <c r="C17" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
+      <c r="D17" s="22">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E17" s="22">
+        <v>0.20833333333333334</v>
+      </c>
       <c r="F17" s="19">
         <v>43206</v>
       </c>
@@ -1164,10 +1152,10 @@
       <c r="C18" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="21">
+      <c r="D18" s="23">
         <v>0.125</v>
       </c>
-      <c r="E18" s="21">
+      <c r="E18" s="23">
         <v>0.25</v>
       </c>
       <c r="F18" s="19">
@@ -1176,15 +1164,15 @@
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="24">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="E19" s="24">
+      <c r="D19" s="23">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E19" s="23">
         <v>0.16666666666666666</v>
       </c>
       <c r="F19" s="19">
@@ -1198,7 +1186,7 @@
       <c r="C20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="22">
+      <c r="D20" s="21">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E20" s="20">
@@ -1210,7 +1198,7 @@
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" s="17" t="s">
         <v>20</v>
@@ -1227,7 +1215,7 @@
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C22" s="17" t="s">
         <v>20</v>
@@ -1244,15 +1232,15 @@
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="24">
+      <c r="D23" s="23">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E23" s="24">
+      <c r="E23" s="23">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F23" s="19">
@@ -1261,15 +1249,15 @@
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C24" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="24">
+      <c r="D24" s="23">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E24" s="24">
+      <c r="E24" s="23">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="F24" s="19">
@@ -1278,15 +1266,15 @@
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C25" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="24">
+      <c r="D25" s="23">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E25" s="24">
+      <c r="E25" s="23">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="F25" s="19">
@@ -1295,15 +1283,15 @@
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C26" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D26" s="24">
+      <c r="D26" s="23">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E26" s="24">
+      <c r="E26" s="23">
         <v>3.125E-2</v>
       </c>
       <c r="F26" s="19">
@@ -1312,15 +1300,15 @@
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C27" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="24">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="E27" s="24">
+      <c r="D27" s="23">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E27" s="23">
         <v>0.125</v>
       </c>
       <c r="F27" s="19">
@@ -1329,81 +1317,85 @@
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C28" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="26">
+      <c r="D28" s="22">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E28" s="26">
+      <c r="E28" s="22">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F28" s="19">
         <v>43209</v>
       </c>
-      <c r="G28" s="27"/>
+      <c r="G28" s="25"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C29" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
+      <c r="D29" s="23">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E29" s="23">
+        <v>0.20833333333333334</v>
+      </c>
       <c r="F29" s="19">
         <v>43209</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C30" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D30" s="24">
+      <c r="D30" s="23">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E30" s="24">
+      <c r="E30" s="23">
         <v>3.125E-2</v>
       </c>
       <c r="F30" s="19">
         <v>43208</v>
       </c>
-      <c r="G30" s="27"/>
+      <c r="G30" s="25"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C31" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D31" s="24">
+      <c r="D31" s="23">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E31" s="24">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="F31" s="28">
+      <c r="E31" s="23">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="F31" s="26">
         <v>43206</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C32" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D32" s="21">
+      <c r="D32" s="23">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E32" s="21">
+      <c r="E32" s="23">
         <v>3.125E-2</v>
       </c>
       <c r="F32" s="19">
@@ -1412,15 +1404,15 @@
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C33" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D33" s="21">
+      <c r="D33" s="23">
         <v>0.29166666666666669</v>
       </c>
-      <c r="E33" s="21">
+      <c r="E33" s="23">
         <v>0.45833333333333331</v>
       </c>
       <c r="F33" s="19">
@@ -1429,15 +1421,15 @@
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C34" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="D34" s="21">
+      <c r="D34" s="23">
         <v>0.125</v>
       </c>
-      <c r="E34" s="21">
+      <c r="E34" s="23">
         <v>0.25</v>
       </c>
       <c r="F34" s="19">
@@ -1446,9 +1438,9 @@
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C35" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" s="24" t="s">
         <v>13</v>
       </c>
       <c r="D35" s="20">
@@ -1463,15 +1455,15 @@
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C36" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="D36" s="21">
+      <c r="D36" s="23">
         <v>3.125E-2</v>
       </c>
-      <c r="E36" s="21">
+      <c r="E36" s="23">
         <v>0.10416666666666667</v>
       </c>
       <c r="F36" s="19">
@@ -1480,15 +1472,15 @@
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C37" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="D37" s="26">
+      <c r="D37" s="22">
         <v>0.75</v>
       </c>
-      <c r="E37" s="26">
+      <c r="E37" s="22">
         <v>0.83333333333333337</v>
       </c>
       <c r="F37" s="19">
@@ -1497,15 +1489,15 @@
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C38" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C38" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D38" s="23">
+      <c r="D38" s="22">
         <v>0.625</v>
       </c>
-      <c r="E38" s="23">
+      <c r="E38" s="22">
         <v>0.625</v>
       </c>
       <c r="F38" s="19">
@@ -1514,15 +1506,15 @@
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C39" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="D39" s="21">
+      <c r="D39" s="23">
         <v>1.3888888888888889E-3</v>
       </c>
-      <c r="E39" s="21">
+      <c r="E39" s="23">
         <v>1.3888888888888889E-3</v>
       </c>
       <c r="F39" s="19">
@@ -1531,48 +1523,60 @@
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C40" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D40" s="26"/>
-      <c r="E40" s="26"/>
+      <c r="D40" s="22">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E40" s="22">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="F40" s="19">
         <v>43208</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="C41" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D41" s="21"/>
-      <c r="E41" s="21"/>
+      <c r="D41" s="23">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="E41" s="23">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="F41" s="19">
         <v>43208</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C42" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
+      <c r="D42" s="22">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E42" s="22">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="F42" s="19">
         <v>43208</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C43" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43" s="24" t="s">
         <v>11</v>
       </c>
       <c r="D43" s="20">
@@ -1587,9 +1591,9 @@
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C44" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C44" s="24" t="s">
         <v>11</v>
       </c>
       <c r="D44" s="20">
@@ -1604,9 +1608,9 @@
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B45" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C45" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45" s="24" t="s">
         <v>11</v>
       </c>
       <c r="D45" s="20">
@@ -1621,9 +1625,9 @@
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="C46" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46" s="24" t="s">
         <v>11</v>
       </c>
       <c r="D46" s="20">
@@ -1638,9 +1642,9 @@
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C47" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C47" s="24" t="s">
         <v>11</v>
       </c>
       <c r="D47" s="20">
@@ -1655,9 +1659,9 @@
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="C48" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" s="24" t="s">
         <v>11</v>
       </c>
       <c r="D48" s="20">
@@ -1672,28 +1676,32 @@
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="C49" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C49" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D49" s="21"/>
-      <c r="E49" s="21"/>
+      <c r="D49" s="23">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E49" s="23">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="F49" s="19">
         <v>43210</v>
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C50" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C50" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="D50" s="21">
+      <c r="D50" s="23">
         <v>3.125E-2</v>
       </c>
-      <c r="E50" s="21">
+      <c r="E50" s="23">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F50" s="19">
@@ -1702,15 +1710,15 @@
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B51" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C51" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C51" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="D51" s="21">
+      <c r="D51" s="23">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="E51" s="21">
+      <c r="E51" s="23">
         <v>3.125E-2</v>
       </c>
       <c r="F51" s="19">
@@ -1719,41 +1727,49 @@
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C52" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C52" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D52" s="21"/>
-      <c r="E52" s="21"/>
+      <c r="D52" s="23">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="E52" s="23">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="F52" s="19">
         <v>43210</v>
       </c>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B53" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="C53" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C53" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D53" s="21"/>
-      <c r="E53" s="21"/>
+      <c r="D53" s="23">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E53" s="23">
+        <v>0.22916666666666666</v>
+      </c>
       <c r="F53" s="19">
         <v>43210</v>
       </c>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C54" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C54" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="D54" s="21">
+      <c r="D54" s="23">
         <v>3.125E-2</v>
       </c>
-      <c r="E54" s="21">
+      <c r="E54" s="23">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F54" s="19">
@@ -1762,15 +1778,15 @@
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B55" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C55" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C55" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="D55" s="21">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="E55" s="21">
+      <c r="D55" s="23">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E55" s="23">
         <v>0.125</v>
       </c>
       <c r="F55" s="19">
@@ -1779,15 +1795,15 @@
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B56" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="C56" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C56" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="D56" s="21">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="E56" s="21">
+      <c r="D56" s="23">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E56" s="23">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F56" s="19">

</xml_diff>